<commit_message>
Se ha añadido numeración a los terminales y no terminales en la tabla de la gramática
</commit_message>
<xml_diff>
--- a/Documentacion Fase 2/Tabla de Análisis Sintáctico.xlsx
+++ b/Documentacion Fase 2/Tabla de Análisis Sintáctico.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\CUNOC\Segundo Semestre 2020\Lenguajes Formales y de Programación\Proyectos\IDE\Documentacion Fase 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DFF255-BC65-473B-9E91-E6E8983D84DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564BCB4C-C760-45FE-9FB8-C3CC5D3E272E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{9F7972A8-781E-4D8B-9578-0A9E6AC1280C}"/>
   </bookViews>
@@ -834,22 +834,131 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B45239-907B-4871-B724-0884F826E03E}">
-  <dimension ref="B1:AL45"/>
+  <dimension ref="A1:AL45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:AL45"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="6.44140625" style="4" customWidth="1"/>
     <col min="2" max="2" width="17.5546875" style="4" customWidth="1"/>
     <col min="3" max="38" width="24.33203125" style="4" customWidth="1"/>
     <col min="39" max="16384" width="11.5546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="4">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4">
+        <v>4</v>
+      </c>
+      <c r="H1" s="4">
+        <v>5</v>
+      </c>
+      <c r="I1" s="4">
+        <v>6</v>
+      </c>
+      <c r="J1" s="4">
+        <v>7</v>
+      </c>
+      <c r="K1" s="4">
+        <v>8</v>
+      </c>
+      <c r="L1" s="4">
+        <v>9</v>
+      </c>
+      <c r="M1" s="4">
+        <v>10</v>
+      </c>
+      <c r="N1" s="4">
+        <v>11</v>
+      </c>
+      <c r="O1" s="4">
+        <v>12</v>
+      </c>
+      <c r="P1" s="4">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="4">
+        <v>14</v>
+      </c>
+      <c r="R1" s="4">
+        <v>15</v>
+      </c>
+      <c r="S1" s="4">
+        <v>16</v>
+      </c>
+      <c r="T1" s="4">
+        <v>17</v>
+      </c>
+      <c r="U1" s="4">
+        <v>18</v>
+      </c>
+      <c r="V1" s="4">
+        <v>19</v>
+      </c>
+      <c r="W1" s="4">
+        <v>20</v>
+      </c>
+      <c r="X1" s="4">
+        <v>21</v>
+      </c>
+      <c r="Y1" s="4">
+        <v>22</v>
+      </c>
+      <c r="Z1" s="4">
+        <v>23</v>
+      </c>
+      <c r="AA1" s="4">
+        <v>24</v>
+      </c>
+      <c r="AB1" s="4">
+        <v>25</v>
+      </c>
+      <c r="AC1" s="4">
+        <v>26</v>
+      </c>
+      <c r="AD1" s="4">
+        <v>27</v>
+      </c>
+      <c r="AE1" s="4">
+        <v>28</v>
+      </c>
+      <c r="AF1" s="4">
+        <v>29</v>
+      </c>
+      <c r="AG1" s="4">
+        <v>30</v>
+      </c>
+      <c r="AH1" s="4">
+        <v>31</v>
+      </c>
+      <c r="AI1" s="4">
+        <v>32</v>
+      </c>
+      <c r="AJ1" s="4">
+        <v>33</v>
+      </c>
+      <c r="AK1" s="4">
+        <v>34</v>
+      </c>
+      <c r="AL1" s="4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
         <v>74</v>
@@ -960,7 +1069,10 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>0</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1003,7 +1115,10 @@
       <c r="AK3" s="6"/>
       <c r="AL3" s="6"/>
     </row>
-    <row r="4" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1046,7 +1161,10 @@
       <c r="AK4" s="6"/>
       <c r="AL4" s="6"/>
     </row>
-    <row r="5" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>2</v>
+      </c>
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
@@ -1105,7 +1223,10 @@
       <c r="AK5" s="6"/>
       <c r="AL5" s="6"/>
     </row>
-    <row r="6" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>3</v>
+      </c>
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1148,7 +1269,10 @@
       <c r="AK6" s="6"/>
       <c r="AL6" s="6"/>
     </row>
-    <row r="7" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>4</v>
+      </c>
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
@@ -1195,7 +1319,10 @@
       <c r="AK7" s="6"/>
       <c r="AL7" s="6"/>
     </row>
-    <row r="8" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>5</v>
+      </c>
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
@@ -1238,7 +1365,10 @@
       <c r="AK8" s="6"/>
       <c r="AL8" s="6"/>
     </row>
-    <row r="9" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>6</v>
+      </c>
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
@@ -1283,7 +1413,10 @@
       <c r="AK9" s="6"/>
       <c r="AL9" s="6"/>
     </row>
-    <row r="10" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>7</v>
+      </c>
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
@@ -1326,7 +1459,10 @@
       <c r="AK10" s="6"/>
       <c r="AL10" s="6"/>
     </row>
-    <row r="11" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>8</v>
+      </c>
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
@@ -1373,7 +1509,10 @@
       <c r="AK11" s="6"/>
       <c r="AL11" s="6"/>
     </row>
-    <row r="12" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>9</v>
+      </c>
       <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
@@ -1428,7 +1567,10 @@
       <c r="AK12" s="6"/>
       <c r="AL12" s="6"/>
     </row>
-    <row r="13" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>10</v>
+      </c>
       <c r="B13" s="2" t="s">
         <v>10</v>
       </c>
@@ -1477,7 +1619,10 @@
       <c r="AK13" s="6"/>
       <c r="AL13" s="6"/>
     </row>
-    <row r="14" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>11</v>
+      </c>
       <c r="B14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1532,7 +1677,10 @@
       <c r="AK14" s="6"/>
       <c r="AL14" s="6"/>
     </row>
-    <row r="15" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>12</v>
+      </c>
       <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
@@ -1581,7 +1729,10 @@
       <c r="AK15" s="6"/>
       <c r="AL15" s="6"/>
     </row>
-    <row r="16" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <v>13</v>
+      </c>
       <c r="B16" s="2" t="s">
         <v>13</v>
       </c>
@@ -1640,7 +1791,10 @@
       <c r="AK16" s="6"/>
       <c r="AL16" s="6"/>
     </row>
-    <row r="17" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <v>14</v>
+      </c>
       <c r="B17" s="2" t="s">
         <v>14</v>
       </c>
@@ -1689,7 +1843,10 @@
       <c r="AK17" s="6"/>
       <c r="AL17" s="6"/>
     </row>
-    <row r="18" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>15</v>
+      </c>
       <c r="B18" s="2" t="s">
         <v>15</v>
       </c>
@@ -1750,7 +1907,10 @@
       <c r="AK18" s="6"/>
       <c r="AL18" s="6"/>
     </row>
-    <row r="19" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <v>16</v>
+      </c>
       <c r="B19" s="2" t="s">
         <v>16</v>
       </c>
@@ -1799,7 +1959,10 @@
       <c r="AK19" s="6"/>
       <c r="AL19" s="6"/>
     </row>
-    <row r="20" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>17</v>
+      </c>
       <c r="B20" s="2" t="s">
         <v>17</v>
       </c>
@@ -1846,7 +2009,10 @@
       <c r="AK20" s="6"/>
       <c r="AL20" s="6"/>
     </row>
-    <row r="21" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>18</v>
+      </c>
       <c r="B21" s="2" t="s">
         <v>18</v>
       </c>
@@ -1889,7 +2055,10 @@
       <c r="AK21" s="6"/>
       <c r="AL21" s="6"/>
     </row>
-    <row r="22" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>19</v>
+      </c>
       <c r="B22" s="2" t="s">
         <v>19</v>
       </c>
@@ -1932,7 +2101,10 @@
       <c r="AK22" s="6"/>
       <c r="AL22" s="6"/>
     </row>
-    <row r="23" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
+        <v>20</v>
+      </c>
       <c r="B23" s="2" t="s">
         <v>20</v>
       </c>
@@ -1981,7 +2153,10 @@
       <c r="AK23" s="6"/>
       <c r="AL23" s="6"/>
     </row>
-    <row r="24" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
+        <v>21</v>
+      </c>
       <c r="B24" s="2" t="s">
         <v>21</v>
       </c>
@@ -2026,7 +2201,10 @@
       <c r="AK24" s="6"/>
       <c r="AL24" s="6"/>
     </row>
-    <row r="25" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4">
+        <v>22</v>
+      </c>
       <c r="B25" s="2" t="s">
         <v>22</v>
       </c>
@@ -2069,7 +2247,10 @@
       <c r="AK25" s="6"/>
       <c r="AL25" s="6"/>
     </row>
-    <row r="26" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
+        <v>23</v>
+      </c>
       <c r="B26" s="2" t="s">
         <v>23</v>
       </c>
@@ -2112,7 +2293,10 @@
       <c r="AK26" s="6"/>
       <c r="AL26" s="6"/>
     </row>
-    <row r="27" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4">
+        <v>24</v>
+      </c>
       <c r="B27" s="2" t="s">
         <v>24</v>
       </c>
@@ -2155,7 +2339,10 @@
       <c r="AK27" s="6"/>
       <c r="AL27" s="6"/>
     </row>
-    <row r="28" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="4">
+        <v>25</v>
+      </c>
       <c r="B28" s="2" t="s">
         <v>25</v>
       </c>
@@ -2198,7 +2385,10 @@
       <c r="AK28" s="6"/>
       <c r="AL28" s="6"/>
     </row>
-    <row r="29" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4">
+        <v>26</v>
+      </c>
       <c r="B29" s="2" t="s">
         <v>26</v>
       </c>
@@ -2241,7 +2431,10 @@
       <c r="AK29" s="6"/>
       <c r="AL29" s="6"/>
     </row>
-    <row r="30" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="4">
+        <v>27</v>
+      </c>
       <c r="B30" s="2" t="s">
         <v>27</v>
       </c>
@@ -2304,7 +2497,10 @@
       <c r="AK30" s="6"/>
       <c r="AL30" s="6"/>
     </row>
-    <row r="31" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="4">
+        <v>28</v>
+      </c>
       <c r="B31" s="2" t="s">
         <v>28</v>
       </c>
@@ -2347,7 +2543,10 @@
       <c r="AK31" s="6"/>
       <c r="AL31" s="6"/>
     </row>
-    <row r="32" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="4">
+        <v>29</v>
+      </c>
       <c r="B32" s="2" t="s">
         <v>29</v>
       </c>
@@ -2400,7 +2599,10 @@
       <c r="AK32" s="6"/>
       <c r="AL32" s="6"/>
     </row>
-    <row r="33" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="4">
+        <v>30</v>
+      </c>
       <c r="B33" s="2" t="s">
         <v>30</v>
       </c>
@@ -2449,7 +2651,10 @@
       <c r="AK33" s="6"/>
       <c r="AL33" s="6"/>
     </row>
-    <row r="34" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="4">
+        <v>31</v>
+      </c>
       <c r="B34" s="2" t="s">
         <v>31</v>
       </c>
@@ -2500,7 +2705,10 @@
       <c r="AK34" s="6"/>
       <c r="AL34" s="6"/>
     </row>
-    <row r="35" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="4">
+        <v>32</v>
+      </c>
       <c r="B35" s="2" t="s">
         <v>32</v>
       </c>
@@ -2545,7 +2753,10 @@
       <c r="AK35" s="6"/>
       <c r="AL35" s="6"/>
     </row>
-    <row r="36" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="4">
+        <v>33</v>
+      </c>
       <c r="B36" s="2" t="s">
         <v>33</v>
       </c>
@@ -2588,7 +2799,10 @@
       <c r="AK36" s="6"/>
       <c r="AL36" s="6"/>
     </row>
-    <row r="37" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="4">
+        <v>34</v>
+      </c>
       <c r="B37" s="2" t="s">
         <v>34</v>
       </c>
@@ -2631,7 +2845,10 @@
       <c r="AK37" s="6"/>
       <c r="AL37" s="6"/>
     </row>
-    <row r="38" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="4">
+        <v>35</v>
+      </c>
       <c r="B38" s="2" t="s">
         <v>35</v>
       </c>
@@ -2674,7 +2891,10 @@
       <c r="AK38" s="6"/>
       <c r="AL38" s="6"/>
     </row>
-    <row r="39" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="4">
+        <v>36</v>
+      </c>
       <c r="B39" s="2" t="s">
         <v>36</v>
       </c>
@@ -2717,7 +2937,10 @@
       <c r="AK39" s="6"/>
       <c r="AL39" s="6"/>
     </row>
-    <row r="40" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="4">
+        <v>37</v>
+      </c>
       <c r="B40" s="2" t="s">
         <v>37</v>
       </c>
@@ -2760,7 +2983,10 @@
       <c r="AK40" s="6"/>
       <c r="AL40" s="6"/>
     </row>
-    <row r="41" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="4">
+        <v>38</v>
+      </c>
       <c r="B41" s="2" t="s">
         <v>38</v>
       </c>
@@ -2803,7 +3029,10 @@
       <c r="AK41" s="6"/>
       <c r="AL41" s="6"/>
     </row>
-    <row r="42" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="4">
+        <v>39</v>
+      </c>
       <c r="B42" s="2" t="s">
         <v>39</v>
       </c>
@@ -2846,7 +3075,10 @@
       <c r="AK42" s="6"/>
       <c r="AL42" s="6"/>
     </row>
-    <row r="43" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="4">
+        <v>40</v>
+      </c>
       <c r="B43" s="2" t="s">
         <v>40</v>
       </c>
@@ -2889,7 +3121,10 @@
       </c>
       <c r="AL43" s="6"/>
     </row>
-    <row r="44" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="4">
+        <v>41</v>
+      </c>
       <c r="B44" s="2" t="s">
         <v>41</v>
       </c>
@@ -2932,7 +3167,10 @@
       <c r="AK44" s="6"/>
       <c r="AL44" s="6"/>
     </row>
-    <row r="45" spans="2:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:38" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="4">
+        <v>42</v>
+      </c>
       <c r="B45" s="2" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
Se ha implementado la tabla de gramática en el código del programa
</commit_message>
<xml_diff>
--- a/Documentacion Fase 2/Tabla de Análisis Sintáctico.xlsx
+++ b/Documentacion Fase 2/Tabla de Análisis Sintáctico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\CUNOC\Segundo Semestre 2020\Lenguajes Formales y de Programación\Proyectos\IDE\Documentacion Fase 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564BCB4C-C760-45FE-9FB8-C3CC5D3E272E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872850BC-2A70-43DB-8740-F86ECE2A1173}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{9F7972A8-781E-4D8B-9578-0A9E6AC1280C}"/>
+    <workbookView xWindow="-8316" yWindow="4308" windowWidth="17280" windowHeight="9072" xr2:uid="{9F7972A8-781E-4D8B-9578-0A9E6AC1280C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -836,8 +836,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B45239-907B-4871-B724-0884F826E03E}">
   <dimension ref="A1:AL45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A45"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="852" topLeftCell="A40" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
El analizador sintáctivo ya funciona, se seguirán haciendo pruebas, únicamente sufrirá cambios en el caso de que se encuentren errores
</commit_message>
<xml_diff>
--- a/Documentacion Fase 2/Tabla de Análisis Sintáctico.xlsx
+++ b/Documentacion Fase 2/Tabla de Análisis Sintáctico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\CUNOC\Segundo Semestre 2020\Lenguajes Formales y de Programación\Proyectos\IDE\Documentacion Fase 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872850BC-2A70-43DB-8740-F86ECE2A1173}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBA8F2B-80E5-40C6-8634-E53E4C61096B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8316" yWindow="4308" windowWidth="17280" windowHeight="9072" xr2:uid="{9F7972A8-781E-4D8B-9578-0A9E6AC1280C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{9F7972A8-781E-4D8B-9578-0A9E6AC1280C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="132">
   <si>
     <t>Codigo</t>
   </si>
@@ -836,9 +836,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B45239-907B-4871-B724-0884F826E03E}">
   <dimension ref="A1:AL45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="852" topLeftCell="A40" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="I45" sqref="I45"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1632" topLeftCell="A30" activePane="bottomLeft"/>
+      <selection activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="AE33" sqref="AE33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1535,9 +1536,7 @@
       <c r="N12" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="O12" s="6" t="s">
-        <v>53</v>
-      </c>
+      <c r="O12" s="6"/>
       <c r="P12" s="6" t="s">
         <v>54</v>
       </c>
@@ -1559,7 +1558,9 @@
       <c r="AB12" s="6"/>
       <c r="AC12" s="6"/>
       <c r="AD12" s="6"/>
-      <c r="AE12" s="6"/>
+      <c r="AE12" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="AF12" s="6"/>
       <c r="AG12" s="6"/>
       <c r="AH12" s="6"/>
@@ -2589,7 +2590,9 @@
       <c r="AB32" s="6"/>
       <c r="AC32" s="6"/>
       <c r="AD32" s="6"/>
-      <c r="AE32" s="6"/>
+      <c r="AE32" s="5" t="s">
+        <v>118</v>
+      </c>
       <c r="AF32" s="5" t="s">
         <v>118</v>
       </c>
@@ -2643,7 +2646,9 @@
       <c r="AB33" s="6"/>
       <c r="AC33" s="6"/>
       <c r="AD33" s="6"/>
-      <c r="AE33" s="6"/>
+      <c r="AE33" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="AF33" s="6"/>
       <c r="AG33" s="6"/>
       <c r="AH33" s="6"/>
@@ -2695,7 +2700,9 @@
       <c r="AB34" s="6"/>
       <c r="AC34" s="6"/>
       <c r="AD34" s="6"/>
-      <c r="AE34" s="6"/>
+      <c r="AE34" s="6" t="s">
+        <v>95</v>
+      </c>
       <c r="AF34" s="6" t="s">
         <v>120</v>
       </c>

</xml_diff>

<commit_message>
Se ha corregido un bug respecto a la agrupación de operaciones
</commit_message>
<xml_diff>
--- a/Documentacion Fase 2/Tabla de Análisis Sintáctico.xlsx
+++ b/Documentacion Fase 2/Tabla de Análisis Sintáctico.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\CUNOC\Segundo Semestre 2020\Lenguajes Formales y de Programación\Proyectos\IDE\Documentacion Fase 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBA8F2B-80E5-40C6-8634-E53E4C61096B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118017A6-CB90-474A-8497-8B0E782BFE09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{9F7972A8-781E-4D8B-9578-0A9E6AC1280C}"/>
+    <workbookView xWindow="16044" yWindow="4212" windowWidth="17280" windowHeight="9072" xr2:uid="{9F7972A8-781E-4D8B-9578-0A9E6AC1280C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="133">
   <si>
     <t>Codigo</t>
   </si>
@@ -422,6 +422,9 @@
   </si>
   <si>
     <t>TokId OpRel NumE</t>
+  </si>
+  <si>
+    <t>( Suma )</t>
   </si>
 </sst>
 </file>
@@ -836,10 +839,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B45239-907B-4871-B724-0884F826E03E}">
   <dimension ref="A1:AL45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1632" topLeftCell="A30" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1632" topLeftCell="A12" activePane="bottomLeft"/>
       <selection activeCell="B11" sqref="B11"/>
-      <selection pane="bottomLeft" activeCell="AE33" sqref="AE33"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1970,7 +1973,7 @@
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6" t="s">
-        <v>43</v>
+        <v>132</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>

</xml_diff>

<commit_message>
Se ha añadido el manual de usuario, y con esto el fin de la documentacióm
</commit_message>
<xml_diff>
--- a/Documentacion Fase 2/Tabla de Análisis Sintáctico.xlsx
+++ b/Documentacion Fase 2/Tabla de Análisis Sintáctico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\CUNOC\Segundo Semestre 2020\Lenguajes Formales y de Programación\Proyectos\IDE\Documentacion Fase 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118017A6-CB90-474A-8497-8B0E782BFE09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2D9F67-ABF5-456D-B6D8-026466EE40C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16044" yWindow="4212" windowWidth="17280" windowHeight="9072" xr2:uid="{9F7972A8-781E-4D8B-9578-0A9E6AC1280C}"/>
+    <workbookView xWindow="5172" yWindow="2712" windowWidth="17280" windowHeight="9072" xr2:uid="{9F7972A8-781E-4D8B-9578-0A9E6AC1280C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -839,10 +839,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B45239-907B-4871-B724-0884F826E03E}">
   <dimension ref="A1:AL45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1632" topLeftCell="A12" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1632" topLeftCell="A9" activePane="bottomLeft"/>
       <selection activeCell="B11" sqref="B11"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>